<commit_message>
fixed errors create and update user
</commit_message>
<xml_diff>
--- a/data/excel/assessment/StudyPeriod.xlsx
+++ b/data/excel/assessment/StudyPeriod.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -462,10 +462,15 @@
           <t>id_dnevnik</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>class_year</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -475,7 +480,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>trimester</t>
+          <t>halfyear</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -485,18 +490,23 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1985862771513643316</t>
+          <t>1985861362764370224</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>10,11,12,13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -506,53 +516,135 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>trimester</t>
+          <t>halfyear</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-06-03</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1985862771513643317</t>
+          <t>1985861362764370225</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>10,11,12,13</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>trimester</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022-09-01</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2022-11-30</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1985862771513643316</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>5,6,7,8,9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>trimester</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2022-12-01</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1985862771513643317</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>5,6,7,8,9</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
         <v>3</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>trimester</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>2023-03-01</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>2023-06-02</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>1985862771513643318</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>5,6,7,8,9</t>
         </is>
       </c>
     </row>

</xml_diff>